<commit_message>
removed hardcoding of M, W, F days on weekly pages
</commit_message>
<xml_diff>
--- a/files/yaml/schedule.xlsx
+++ b/files/yaml/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duttas\Desktop\Programming\CanvasCrafter\files\yaml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vihdutta\CanvasCrafter\files\yaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4F3159-796C-4722-A06E-249737CB1E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818FFDA-DD7B-44D3-AC05-5DA55CAA2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FA25_Weeks" sheetId="9" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -619,6 +630,21 @@
   </si>
   <si>
     <t>Study for Final Exam</t>
+  </si>
+  <si>
+    <t>Nothing! Done with school!</t>
+  </si>
+  <si>
+    <t>Still nothing.</t>
+  </si>
+  <si>
+    <t>10/3</t>
+  </si>
+  <si>
+    <t>END1</t>
+  </si>
+  <si>
+    <t>END2</t>
   </si>
 </sst>
 </file>
@@ -716,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -986,11 +1012,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1338,6 +1375,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1700,17 +1741,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N49"/>
+  <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="11" bestFit="1" customWidth="1"/>
@@ -1758,10 +1799,10 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="121">
+      <c r="B3" s="123">
         <v>1</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="126" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="25" t="s">
@@ -1788,8 +1829,8 @@
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="122"/>
-      <c r="C4" s="125"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="127"/>
       <c r="D4" s="13" t="s">
         <v>67</v>
       </c>
@@ -1815,8 +1856,8 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="123"/>
-      <c r="C5" s="125"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="127"/>
       <c r="D5" s="13" t="s">
         <v>68</v>
       </c>
@@ -1844,10 +1885,10 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="121">
+      <c r="B6" s="123">
         <v>2</v>
       </c>
-      <c r="C6" s="125"/>
+      <c r="C6" s="127"/>
       <c r="D6" s="110" t="s">
         <v>26</v>
       </c>
@@ -1871,8 +1912,8 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="122"/>
-      <c r="C7" s="126"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="128"/>
       <c r="D7" s="86" t="s">
         <v>69</v>
       </c>
@@ -1898,8 +1939,8 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="123"/>
-      <c r="C8" s="127" t="s">
+      <c r="B8" s="125"/>
+      <c r="C8" s="129" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -1931,10 +1972,10 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="121">
+      <c r="B9" s="123">
         <v>3</v>
       </c>
-      <c r="C9" s="128"/>
+      <c r="C9" s="130"/>
       <c r="D9" s="6" t="s">
         <v>71</v>
       </c>
@@ -1962,8 +2003,8 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="122"/>
-      <c r="C10" s="128"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="6" t="s">
         <v>72</v>
       </c>
@@ -1989,8 +2030,8 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="123"/>
-      <c r="C11" s="128"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
@@ -2020,10 +2061,10 @@
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="121">
+      <c r="B12" s="123">
         <v>4</v>
       </c>
-      <c r="C12" s="128"/>
+      <c r="C12" s="130"/>
       <c r="D12" s="6" t="s">
         <v>73</v>
       </c>
@@ -2051,8 +2092,8 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="122"/>
-      <c r="C13" s="128"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="6" t="s">
         <v>74</v>
       </c>
@@ -2078,8 +2119,8 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="123"/>
-      <c r="C14" s="128"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="6" t="s">
         <v>75</v>
       </c>
@@ -2109,10 +2150,10 @@
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="121">
+      <c r="B15" s="123">
         <v>5</v>
       </c>
-      <c r="C15" s="128"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="6" t="s">
         <v>76</v>
       </c>
@@ -2138,8 +2179,8 @@
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="122"/>
-      <c r="C16" s="128"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="6" t="s">
         <v>77</v>
       </c>
@@ -2165,8 +2206,8 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="123"/>
-      <c r="C17" s="128"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
@@ -2196,10 +2237,10 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="121">
+      <c r="B18" s="123">
         <v>6</v>
       </c>
-      <c r="C18" s="128"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="6" t="s">
         <v>78</v>
       </c>
@@ -2225,8 +2266,8 @@
       <c r="M18" s="4"/>
     </row>
     <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="122"/>
-      <c r="C19" s="129"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="98" t="s">
         <v>79</v>
       </c>
@@ -2252,8 +2293,8 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="123"/>
-      <c r="C20" s="130" t="s">
+      <c r="B20" s="125"/>
+      <c r="C20" s="132" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="33" t="s">
@@ -2285,10 +2326,10 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="121">
+      <c r="B21" s="123">
         <v>7</v>
       </c>
-      <c r="C21" s="131"/>
+      <c r="C21" s="133"/>
       <c r="D21" s="16" t="s">
         <v>81</v>
       </c>
@@ -2314,8 +2355,8 @@
       <c r="M21" s="4"/>
     </row>
     <row r="22" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="122"/>
-      <c r="C22" s="132"/>
+      <c r="B22" s="124"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="88" t="s">
         <v>82</v>
       </c>
@@ -2339,8 +2380,8 @@
       <c r="M22" s="4"/>
     </row>
     <row r="23" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="123"/>
-      <c r="C23" s="133" t="s">
+      <c r="B23" s="125"/>
+      <c r="C23" s="135" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="40" t="s">
@@ -2372,10 +2413,10 @@
       <c r="M23" s="4"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="121">
+      <c r="B24" s="123">
         <v>8</v>
       </c>
-      <c r="C24" s="134"/>
+      <c r="C24" s="136"/>
       <c r="D24" s="108" t="s">
         <v>26</v>
       </c>
@@ -2397,8 +2438,8 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="122"/>
-      <c r="C25" s="134"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="19" t="s">
         <v>84</v>
       </c>
@@ -2424,8 +2465,8 @@
       <c r="M25" s="4"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="123"/>
-      <c r="C26" s="134"/>
+      <c r="B26" s="125"/>
+      <c r="C26" s="136"/>
       <c r="D26" s="19" t="s">
         <v>26</v>
       </c>
@@ -2453,10 +2494,10 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="121">
+      <c r="B27" s="123">
         <v>9</v>
       </c>
-      <c r="C27" s="134"/>
+      <c r="C27" s="136"/>
       <c r="D27" s="19" t="s">
         <v>85</v>
       </c>
@@ -2483,8 +2524,8 @@
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="122"/>
-      <c r="C28" s="134"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="136"/>
       <c r="D28" s="19" t="s">
         <v>86</v>
       </c>
@@ -2511,8 +2552,8 @@
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="123"/>
-      <c r="C29" s="134"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="136"/>
       <c r="D29" s="19" t="s">
         <v>87</v>
       </c>
@@ -2543,10 +2584,10 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="121">
+      <c r="B30" s="123">
         <v>10</v>
       </c>
-      <c r="C30" s="134"/>
+      <c r="C30" s="136"/>
       <c r="D30" s="19" t="s">
         <v>88</v>
       </c>
@@ -2573,8 +2614,8 @@
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="122"/>
-      <c r="C31" s="134"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="136"/>
       <c r="D31" s="19" t="s">
         <v>89</v>
       </c>
@@ -2601,8 +2642,8 @@
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="2:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="123"/>
-      <c r="C32" s="135"/>
+      <c r="B32" s="125"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="45" t="s">
         <v>26</v>
       </c>
@@ -2631,10 +2672,10 @@
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="121">
+      <c r="B33" s="123">
         <v>11</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="138" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="47" t="s">
@@ -2663,8 +2704,8 @@
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="122"/>
-      <c r="C34" s="137"/>
+      <c r="B34" s="124"/>
+      <c r="C34" s="139"/>
       <c r="D34" s="8" t="s">
         <v>91</v>
       </c>
@@ -2691,8 +2732,8 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="123"/>
-      <c r="C35" s="137"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="139"/>
       <c r="D35" s="8" t="s">
         <v>92</v>
       </c>
@@ -2723,10 +2764,10 @@
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="121">
+      <c r="B36" s="123">
         <v>12</v>
       </c>
-      <c r="C36" s="137"/>
+      <c r="C36" s="139"/>
       <c r="D36" s="8" t="s">
         <v>93</v>
       </c>
@@ -2753,8 +2794,8 @@
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="122"/>
-      <c r="C37" s="137"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="139"/>
       <c r="D37" s="8" t="s">
         <v>94</v>
       </c>
@@ -2781,8 +2822,8 @@
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="123"/>
-      <c r="C38" s="137"/>
+      <c r="B38" s="125"/>
+      <c r="C38" s="139"/>
       <c r="D38" s="8" t="s">
         <v>95</v>
       </c>
@@ -2815,10 +2856,10 @@
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="121">
+      <c r="B39" s="123">
         <v>13</v>
       </c>
-      <c r="C39" s="137"/>
+      <c r="C39" s="139"/>
       <c r="D39" s="8" t="s">
         <v>96</v>
       </c>
@@ -2845,8 +2886,8 @@
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="122"/>
-      <c r="C40" s="137"/>
+      <c r="B40" s="124"/>
+      <c r="C40" s="139"/>
       <c r="D40" s="8" t="s">
         <v>97</v>
       </c>
@@ -2873,8 +2914,8 @@
       <c r="N40" s="1"/>
     </row>
     <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="123"/>
-      <c r="C41" s="138"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="140"/>
       <c r="D41" s="52" t="s">
         <v>26</v>
       </c>
@@ -2905,10 +2946,10 @@
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="121">
+      <c r="B42" s="123">
         <v>14</v>
       </c>
-      <c r="C42" s="139" t="s">
+      <c r="C42" s="141" t="s">
         <v>31</v>
       </c>
       <c r="D42" s="56" t="s">
@@ -2939,8 +2980,8 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="122"/>
-      <c r="C43" s="140"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="142"/>
       <c r="D43" s="110" t="s">
         <v>26</v>
       </c>
@@ -2951,7 +2992,7 @@
       <c r="F43" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="119" t="s">
+      <c r="G43" s="121" t="s">
         <v>104</v>
       </c>
       <c r="H43" s="115" t="s">
@@ -2965,8 +3006,8 @@
       <c r="N43" s="1"/>
     </row>
     <row r="44" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="123"/>
-      <c r="C44" s="140"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="142"/>
       <c r="D44" s="110" t="s">
         <v>26</v>
       </c>
@@ -2977,7 +3018,7 @@
       <c r="F44" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="120"/>
+      <c r="G44" s="122"/>
       <c r="H44" s="115" t="s">
         <v>26</v>
       </c>
@@ -2989,10 +3030,10 @@
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="121">
+      <c r="B45" s="123">
         <v>15</v>
       </c>
-      <c r="C45" s="140"/>
+      <c r="C45" s="142"/>
       <c r="D45" s="23" t="s">
         <v>99</v>
       </c>
@@ -3019,8 +3060,8 @@
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="122"/>
-      <c r="C46" s="140"/>
+      <c r="B46" s="124"/>
+      <c r="C46" s="142"/>
       <c r="D46" s="23" t="s">
         <v>100</v>
       </c>
@@ -3047,8 +3088,8 @@
       <c r="N46" s="1"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="123"/>
-      <c r="C47" s="140"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="142"/>
       <c r="D47" s="23" t="s">
         <v>101</v>
       </c>
@@ -3077,10 +3118,10 @@
       <c r="N47" s="1"/>
     </row>
     <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="121">
+      <c r="B48" s="123">
         <v>16</v>
       </c>
-      <c r="C48" s="141"/>
+      <c r="C48" s="143"/>
       <c r="D48" s="62" t="s">
         <v>106</v>
       </c>
@@ -3109,7 +3150,7 @@
       <c r="N48" s="1"/>
     </row>
     <row r="49" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="142"/>
+      <c r="B49" s="144"/>
       <c r="C49" s="90"/>
       <c r="D49" s="90"/>
       <c r="E49" s="90">
@@ -3129,6 +3170,49 @@
         <v>169</v>
       </c>
       <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E50" s="119">
+        <v>46368</v>
+      </c>
+      <c r="G50" s="120" t="s">
+        <v>173</v>
+      </c>
+      <c r="L50" s="81" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E51" s="119">
+        <v>46369</v>
+      </c>
+      <c r="G51" s="120" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="L51" s="81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D52" s="11"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="1"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D53" s="11"/>
+      <c r="G53" s="81"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="1"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
made <3 day weeks stretch to fit
</commit_message>
<xml_diff>
--- a/files/yaml/schedule.xlsx
+++ b/files/yaml/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vihdutta\CanvasCrafter\files\yaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818FFDA-DD7B-44D3-AC05-5DA55CAA2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70630215-8934-4EA8-BCD6-BC71FCEFA0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FA25_Weeks" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="172">
   <si>
     <t>Date</t>
   </si>
@@ -635,16 +635,7 @@
     <t>Nothing! Done with school!</t>
   </si>
   <si>
-    <t>Still nothing.</t>
-  </si>
-  <si>
-    <t>10/3</t>
-  </si>
-  <si>
     <t>END1</t>
-  </si>
-  <si>
-    <t>END2</t>
   </si>
 </sst>
 </file>
@@ -1743,28 +1734,28 @@
   </sheetPr>
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L51" sqref="D51:L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="4.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="81" customWidth="1"/>
-    <col min="12" max="12" width="61.5703125" style="81" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="4.5546875" style="81" customWidth="1"/>
+    <col min="12" max="12" width="61.5546875" style="81" customWidth="1"/>
     <col min="13" max="13" width="78" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" s="2" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="85" t="s">
         <v>65</v>
       </c>
@@ -1798,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="123">
         <v>1</v>
       </c>
@@ -1828,7 +1819,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="124"/>
       <c r="C4" s="127"/>
       <c r="D4" s="13" t="s">
@@ -1855,7 +1846,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="125"/>
       <c r="C5" s="127"/>
       <c r="D5" s="13" t="s">
@@ -1884,7 +1875,7 @@
       </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="123">
         <v>2</v>
       </c>
@@ -1911,7 +1902,7 @@
       <c r="L6" s="67"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="124"/>
       <c r="C7" s="128"/>
       <c r="D7" s="86" t="s">
@@ -1938,7 +1929,7 @@
       </c>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="125"/>
       <c r="C8" s="129" t="s">
         <v>28</v>
@@ -1971,7 +1962,7 @@
       </c>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="123">
         <v>3</v>
       </c>
@@ -2002,7 +1993,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="124"/>
       <c r="C10" s="130"/>
       <c r="D10" s="6" t="s">
@@ -2029,7 +2020,7 @@
       </c>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="125"/>
       <c r="C11" s="130"/>
       <c r="D11" s="6" t="s">
@@ -2060,7 +2051,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="123">
         <v>4</v>
       </c>
@@ -2091,7 +2082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="124"/>
       <c r="C13" s="130"/>
       <c r="D13" s="6" t="s">
@@ -2118,7 +2109,7 @@
       </c>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="125"/>
       <c r="C14" s="130"/>
       <c r="D14" s="6" t="s">
@@ -2149,7 +2140,7 @@
       </c>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="123">
         <v>5</v>
       </c>
@@ -2178,7 +2169,7 @@
       </c>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="124"/>
       <c r="C16" s="130"/>
       <c r="D16" s="6" t="s">
@@ -2205,7 +2196,7 @@
       </c>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="125"/>
       <c r="C17" s="130"/>
       <c r="D17" s="6" t="s">
@@ -2236,7 +2227,7 @@
       </c>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="123">
         <v>6</v>
       </c>
@@ -2265,7 +2256,7 @@
       </c>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="124"/>
       <c r="C19" s="131"/>
       <c r="D19" s="98" t="s">
@@ -2292,7 +2283,7 @@
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="125"/>
       <c r="C20" s="132" t="s">
         <v>32</v>
@@ -2325,7 +2316,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="123">
         <v>7</v>
       </c>
@@ -2354,7 +2345,7 @@
       </c>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="124"/>
       <c r="C22" s="134"/>
       <c r="D22" s="88" t="s">
@@ -2379,7 +2370,7 @@
       </c>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="125"/>
       <c r="C23" s="135" t="s">
         <v>29</v>
@@ -2412,7 +2403,7 @@
       </c>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="123">
         <v>8</v>
       </c>
@@ -2437,7 +2428,7 @@
       <c r="L24" s="67"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="124"/>
       <c r="C25" s="136"/>
       <c r="D25" s="19" t="s">
@@ -2464,7 +2455,7 @@
       </c>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="125"/>
       <c r="C26" s="136"/>
       <c r="D26" s="19" t="s">
@@ -2493,7 +2484,7 @@
       </c>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="123">
         <v>9</v>
       </c>
@@ -2523,7 +2514,7 @@
       <c r="M27" s="4"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="124"/>
       <c r="C28" s="136"/>
       <c r="D28" s="19" t="s">
@@ -2551,7 +2542,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="125"/>
       <c r="C29" s="136"/>
       <c r="D29" s="19" t="s">
@@ -2583,7 +2574,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="123">
         <v>10</v>
       </c>
@@ -2613,7 +2604,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="124"/>
       <c r="C31" s="136"/>
       <c r="D31" s="19" t="s">
@@ -2641,7 +2632,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="2:14" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="125"/>
       <c r="C32" s="137"/>
       <c r="D32" s="45" t="s">
@@ -2671,7 +2662,7 @@
       <c r="M32" s="4"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="123">
         <v>11</v>
       </c>
@@ -2703,7 +2694,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="124"/>
       <c r="C34" s="139"/>
       <c r="D34" s="8" t="s">
@@ -2731,7 +2722,7 @@
       <c r="M34" s="4"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="125"/>
       <c r="C35" s="139"/>
       <c r="D35" s="8" t="s">
@@ -2763,7 +2754,7 @@
       <c r="M35" s="4"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="123">
         <v>12</v>
       </c>
@@ -2793,7 +2784,7 @@
       <c r="M36" s="4"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="124"/>
       <c r="C37" s="139"/>
       <c r="D37" s="8" t="s">
@@ -2821,7 +2812,7 @@
       <c r="M37" s="78"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="125"/>
       <c r="C38" s="139"/>
       <c r="D38" s="8" t="s">
@@ -2855,7 +2846,7 @@
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="123">
         <v>13</v>
       </c>
@@ -2885,7 +2876,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="124"/>
       <c r="C40" s="139"/>
       <c r="D40" s="8" t="s">
@@ -2913,7 +2904,7 @@
       <c r="M40" s="4"/>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="125"/>
       <c r="C41" s="140"/>
       <c r="D41" s="52" t="s">
@@ -2945,7 +2936,7 @@
       <c r="M41" s="4"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="123">
         <v>14</v>
       </c>
@@ -2979,7 +2970,7 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="124"/>
       <c r="C43" s="142"/>
       <c r="D43" s="110" t="s">
@@ -3005,7 +2996,7 @@
       <c r="M43" s="4"/>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="125"/>
       <c r="C44" s="142"/>
       <c r="D44" s="110" t="s">
@@ -3029,7 +3020,7 @@
       <c r="M44" s="4"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="123">
         <v>15</v>
       </c>
@@ -3059,7 +3050,7 @@
       <c r="M45" s="4"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="124"/>
       <c r="C46" s="142"/>
       <c r="D46" s="23" t="s">
@@ -3087,7 +3078,7 @@
       <c r="M46" s="4"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="125"/>
       <c r="C47" s="142"/>
       <c r="D47" s="23" t="s">
@@ -3117,7 +3108,7 @@
       <c r="M47" s="4"/>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="123">
         <v>16</v>
       </c>
@@ -3149,7 +3140,7 @@
       </c>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="144"/>
       <c r="C49" s="90"/>
       <c r="D49" s="90"/>
@@ -3171,32 +3162,22 @@
       </c>
       <c r="M49" s="4"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E50" s="119">
         <v>46368</v>
       </c>
       <c r="G50" s="120" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L50" s="81" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="119">
-        <v>46369</v>
-      </c>
-      <c r="G51" s="120" t="s">
-        <v>174</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L51" s="81" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E51" s="119"/>
+      <c r="G51" s="120"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D52" s="11"/>
       <c r="G52" s="81"/>
       <c r="H52" s="81"/>
@@ -3205,7 +3186,7 @@
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D53" s="11"/>
       <c r="G53" s="81"/>
       <c r="H53" s="81"/>

</xml_diff>